<commit_message>
Fix failed urls excel
</commit_message>
<xml_diff>
--- a/excel-files/descriptions/description-html.xlsx
+++ b/excel-files/descriptions/description-html.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffe\Documents\SILABUZ\nataly\29-agosto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffe\Documents\SILABUZ\PRODUCCION\13-set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EECE5E5C-2031-433C-8611-35158B6A766F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C41AD572-625F-4678-85FA-22B45726116B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5146D8D-5D62-41B7-BB1D-92B86E77855F}"/>
   </bookViews>
@@ -36,63 +36,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>columna_html</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt; Bolsillo frontal con cierre&lt;li&gt; Bolsillo posterior con cierre&lt;li&gt; Bolsillo interno con cierre&lt;li&gt; Correa regulable&lt;li&gt; Respaldar acolchado&lt;li&gt; Forro interno reciclado&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;h2&gt;Filtro de Grifo Giratorio para Cocina Anti-Splash&lt;/h2&gt;_x000D_
+&lt;h3&gt;Caracter&amp;iacute;sticas:&lt;/h3&gt;_x000D_
+&lt;ul&gt;_x000D_
+&lt;li&gt;Cabezal para salpicaduras.&lt;/li&gt;_x000D_
+&lt;li&gt;Colores: Variados.&lt;/li&gt;_x000D_
+&lt;li&gt;Material: PP.&lt;/li&gt;_x000D_
+&lt;li&gt;Tama&amp;ntilde;o: 6.5 x 2.5 x 5 cm.&lt;/li&gt;_x000D_
+&lt;li&gt;Flexibilidad 360&amp;deg;.&lt;/li&gt;_x000D_
+&lt;li&gt;F&amp;aacute;cil instalaci&amp;oacute;n.&lt;/li&gt;_x000D_
+&lt;/ul&gt;_x000D_
+&lt;h3&gt;Descripci&amp;oacute;n:&lt;/h3&gt;_x000D_
+&lt;p&gt;&amp;iexcl;Dile adi&amp;oacute;s a las salpicaduras de agua al lavar!&lt;/p&gt;_x000D_
+&lt;p&gt;Nuestro filtro de agua ser&amp;aacute; tu mejor aliado en la cocina y/o ba&amp;ntilde;o.&lt;/p&gt;_x000D_
+&lt;p&gt;Ahorro de agua: Ahorrar&amp;aacute;s entre un 30 - 70 % a comparaci&amp;oacute;n de burbujeadores est&amp;aacute;ndar. Podr&amp;aacute;s aumentar la presi&amp;oacute;n del agua, garantizando una mejor limpieza.&lt;/p&gt;_x000D_
+&lt;p&gt;Giro de 360&amp;deg;: Cabeza giratoria que permite f&amp;aacute;cil alcance en todo el fregadero.&lt;/p&gt;_x000D_
+&lt;p&gt;Dise&amp;ntilde;o f&amp;aacute;cil de instalar y limpiar.&lt;/p&gt;_x000D_
+&lt;p&gt;Ideal para cocina, lavaderos.&lt;/p&gt;_x000D_
+&lt;h4&gt;CC GROUP&lt;/h4&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Asas de mano&lt;li&gt; Bolsillos interiores con cierre&lt;li&gt; Bolsillo frontal con cierre&lt;li&gt; Bolsillo con cierre en respaldar&lt;li&gt; Bolsillos laterales con cierre&lt;li&gt; Bolsillo lateral especial para zapatillas&lt;li&gt; Correa regulable&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Mug curvo de cerámica new bone china con divertido diseño impreso.&lt;/p&gt;
+  &lt;ul&gt;
+  &lt;li&gt;Cuenta con una capacidad de 350 ml.&lt;/li&gt;
+  &lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt; Bolsillo exterior frontal con cierre&lt;li&gt; Bolsillo exterior posterior con cierre&lt;li&gt; Bolsillos laterales con elástico&lt;li&gt; Cintas de compresión laterales&lt;li&gt; Correa regulable para hombro&lt;li&gt; Asa de mano&lt;li&gt; Bolsillos internos&lt;li&gt; Gancho para llaves&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt; Bolsillo interno simple&lt;li&gt; Bolsillos frontales con cierre&lt;li&gt; Bolsillo posterior con cierre&lt;li&gt; Correa regulable&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt; Interior térmico&lt;li&gt; Asa de mano&lt;li&gt; Correa para hombro regulable&lt;li&gt; Cierre exterior&lt;li&gt; Bolsillo de malla&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt; Asas de mano&lt;li&gt; Compartimiento principal con cierre&lt;li&gt; Bolsillos externos con cierre&lt;li&gt; Correa regulable para hombros&lt;li&gt; Bolsillos internos&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maleta con sistema de 4 ruedas multidirecionales con giro de 360°&lt;li&gt;Asa paralela superior para traslado&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;li&gt;Interiores de equipaje totalmente forrado&lt;li&gt;Bolsillo interno de cierre con malla&lt;li&gt;Correas elásticas de embalaje para mantener las prendas seguras&lt;li&gt;Cierre expansor&lt;li&gt;Cierre con sistema de seguridad para candado&lt;li&gt;Cerraduras con sistema TSA&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt; Bolsillo frontal con broche&lt;li&gt; Bolsillo posterior con cierre&lt;li&gt; Bolsillos internos simples&lt;li&gt; Bolsillo interno con cierre&lt;li&gt; Bolsillos laterales con cierres&lt;li&gt; Respaldar acolchado&lt;li&gt; Correa regulable&lt;li&gt; Forro interno reciclado&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt; Asas para hombro&lt;li&gt; Compartimiento principal con cierre&lt;li&gt; Bolsillos exteriores&lt;li&gt; Bolsillos internos simples&lt;li&gt; Bolsillo interior con cierre&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt; Maleta con sistema de 8 ruedas multidirecionales con giro de 360°&lt;li&gt;Asa paralela de mano superior para traslado&lt;li&gt;Asa de mano lateral para carga y levantamiento&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;li&gt;Interiores de equipaje totalmente forrado&lt;li&gt;Bolsillos internos de malla con cierre&lt;li&gt;Compartimento frontal que se abre con accesorio ubicado en la parte superior&lt;li&gt;Accesorio USB y puerto C&lt;li&gt;Portalaptop&lt;li&gt;Correas elásticas de embalaje internas para mantener las prendas seguras&lt;li&gt;Cerraduras con sistema TSA&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maleta con sistema de 8 ruedas multidirecionales con giro de 360°&lt;li&gt;Asa paralela de mano superior para traslado&lt;li&gt;Asa de mano lateral para carga y levantamiento&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;li&gt;Interiores de equipaje totalmente forrado&lt;li&gt;Bolsillos internos de malla con cierre&lt;li&gt;Compartimento frontal que se abre con accesorio ubicado en la parte superior&lt;li&gt;Accesorio USB y puerto C&lt;li&gt;Portalaptop&lt;li&gt;Correas elásticas de embalaje internas para mantener las prendas seguras&lt;li&gt;Cerraduras con sistema TSA&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maleta con sistema de 4 ruedas multidirecionales con giro de 360°&lt;li&gt;Asa paralela superior para traslado&lt;li&gt;Asa de mano superior y lateral para carga y levantamiento ( 28” Y 24”)&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;li&gt;Interiores de equipaje totalmente forrado&lt;li&gt;Bolsillo interno de cierre con malla&lt;li&gt;Correas elásticas de embalaje para mantener las prendas seguras&lt;li&gt;Cierre expansor&lt;li&gt;Cierre con sistema de seguridad para candado&lt;li&gt;Cerraduras con sistema TSA&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maleta con sistema de 4 ruedas multidirecionales con giro de 360°&lt;li&gt;Asa paralela superior para traslado&lt;li&gt;Asa de mano superior y lateral para carga y levantamiento (28” Y 24”)&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;li&gt;Interiores de equipaje totalmente forrado&lt;li&gt;Bolsillo interno de cierre con malla&lt;li&gt;Correas elásticas de embalaje para mantener las prendas seguras&lt;li&gt;Cierre expansor&lt;li&gt;Cierre con sistema de seguridad para candado&lt;li&gt;Cerraduras con sistema TSA&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Maleta con sistema de 4 ruedas multidireccionales con giro de 360°_x000D_&lt;li&gt;Asa paralela superior para traslado_x000D_&lt;li&gt;Asa de mano superior y lateral para carga y levantamiento_x000D_&lt;li&gt;Botón de seguridad en asa retráctil de aluminio_x000D_&lt;li&gt;Interiores de equipaje totalmente forrado_x000D_&lt;li&gt;Bolsillo interno de cierre_x000D_&lt;li&gt;Correas de embalaje para mantener las prendas seguras_x000D_&lt;li&gt;Cierre expansor_x000D_&lt;li&gt;Cierre con sistema de seguridad para candado_x000D_&lt;li&gt;Cierre con sistema TSA*_x000D_&lt;li&gt;Compartimiento exterior de cierre_x000D_&lt;li&gt;Bolsillo frontal de cierre&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Un compartimiento principal con cierre&lt;li&gt;Bolsillo interno con cierre&lt;li&gt;Bolsillo frontal con cierre&lt;li&gt;Bolsillo posterior con cierre&lt;li&gt;Correa regulable&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal&lt;li&gt;Cerraduras con sistema TSA&lt;li&gt;Bolsillos internos&lt;li&gt;Bolsillos organizadores internos&lt;li&gt;Asa paralela superior para traslado&lt;li&gt;Botón de seguridad en asa retráctil de aluminio&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt;Bolsillo frontal con cierre&lt;li&gt;Correa regulable&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Compartimiento principal con cierre&lt;li&gt;Asa de mano&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Individual de PVC de color liso&lt;/p&gt;
+ &lt;ul&gt;
+ &lt;li&gt;Tiene un tamaño de 44x29 cm&lt;/li&gt;
+ &lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -465,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D905A2E3-ECD2-45DA-85CB-0EE3959B2D62}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A43"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,202 +468,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>